<commit_message>
Updating charts and adding test cases
</commit_message>
<xml_diff>
--- a/User Stories-Acceptance Criteria-Test Cases/Acceptance Criteria - Code Avengers - Book Buddy.xlsx
+++ b/User Stories-Acceptance Criteria-Test Cases/Acceptance Criteria - Code Avengers - Book Buddy.xlsx
@@ -427,12 +427,12 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> the system will generate recommendations based off no input</t>
+      <t xml:space="preserve"> the system will generate recommendations based off genres liked</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">
--The system will have a way to return recommendations with no input</t>
+-The system will have a way to return recommendations with genres only</t>
   </si>
   <si>
     <t>US7</t>

</xml_diff>